<commit_message>
Add lead field to TicketOrder
</commit_message>
<xml_diff>
--- a/song_signup/tests/tickchak-orders-extended.xlsx
+++ b/song_signup/tests/tickchak-orders-extended.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="116">
   <si>
     <t>מספר הזמנה</t>
   </si>
@@ -276,6 +276,9 @@
   </si>
   <si>
     <t>סולימאן1610@walla.co.il</t>
+  </si>
+  <si>
+    <t>added-lead</t>
   </si>
   <si>
     <t>קופה רושמת</t>
@@ -559,28 +562,28 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -762,9 +765,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -844,7 +847,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -872,10 +875,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1131,9 +1134,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -1421,7 +1424,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1449,10 +1452,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2403,13 +2406,15 @@
       <c r="L12" s="7">
         <v>0</v>
       </c>
-      <c r="M12" s="10"/>
+      <c r="M12" t="s" s="8">
+        <v>69</v>
+      </c>
       <c r="N12" s="10"/>
       <c r="O12" t="s" s="9">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P12" t="s" s="9">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q12" t="s" s="9">
         <v>31</v>
@@ -2418,7 +2423,7 @@
         <v>0</v>
       </c>
       <c r="S12" t="s" s="8">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="T12" s="7">
         <v>23218161571801</v>
@@ -2430,19 +2435,19 @@
         <v>11017601</v>
       </c>
       <c r="B13" t="s" s="8">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C13" t="s" s="9">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D13" t="s" s="9">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E13" t="s" s="8">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F13" t="s" s="9">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" t="s" s="9">
@@ -2463,10 +2468,10 @@
       <c r="M13" s="10"/>
       <c r="N13" s="10"/>
       <c r="O13" t="s" s="9">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P13" t="s" s="9">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q13" t="s" s="9">
         <v>31</v>
@@ -2475,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="S13" t="s" s="8">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="T13" s="7">
         <v>23218829632344</v>
@@ -2487,19 +2492,19 @@
         <v>11017601</v>
       </c>
       <c r="B14" t="s" s="8">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s" s="9">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s" s="9">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s" s="8">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F14" t="s" s="9">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" t="s" s="9">
@@ -2520,10 +2525,10 @@
       <c r="M14" s="10"/>
       <c r="N14" s="10"/>
       <c r="O14" t="s" s="9">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P14" t="s" s="9">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="Q14" t="s" s="9">
         <v>31</v>
@@ -2532,7 +2537,7 @@
         <v>0</v>
       </c>
       <c r="S14" t="s" s="8">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="T14" s="7">
         <v>23217857698402</v>
@@ -2544,19 +2549,19 @@
         <v>11017747</v>
       </c>
       <c r="B15" t="s" s="8">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C15" t="s" s="9">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D15" t="s" s="9">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s" s="8">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s" s="9">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="G15" s="10"/>
       <c r="H15" t="s" s="9">
@@ -2589,7 +2594,7 @@
         <v>0</v>
       </c>
       <c r="S15" t="s" s="8">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="T15" s="7">
         <v>23220845161256</v>
@@ -2601,19 +2606,19 @@
         <v>11024153</v>
       </c>
       <c r="B16" t="s" s="8">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s" s="8">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s" s="8">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E16" t="s" s="8">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s" s="8">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="G16" s="10"/>
       <c r="H16" t="s" s="9">
@@ -2627,7 +2632,9 @@
       </c>
       <c r="K16" s="10"/>
       <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
+      <c r="M16" t="s" s="8">
+        <v>28</v>
+      </c>
       <c r="N16" s="10"/>
       <c r="O16" s="10"/>
       <c r="P16" s="10"/>
@@ -2642,19 +2649,19 @@
         <v>11029561</v>
       </c>
       <c r="B17" t="s" s="8">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C17" t="s" s="8">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D17" t="s" s="8">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s" s="8">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F17" t="s" s="8">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G17" s="10"/>
       <c r="H17" t="s" s="9">
@@ -2668,7 +2675,9 @@
       </c>
       <c r="K17" s="10"/>
       <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
+      <c r="M17" t="s" s="8">
+        <v>28</v>
+      </c>
       <c r="N17" s="10"/>
       <c r="O17" s="10"/>
       <c r="P17" s="10"/>
@@ -2683,19 +2692,19 @@
         <v>11029376</v>
       </c>
       <c r="B18" t="s" s="8">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C18" t="s" s="9">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D18" t="s" s="9">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E18" t="s" s="8">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F18" t="s" s="9">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G18" s="10"/>
       <c r="H18" t="s" s="9">
@@ -2724,19 +2733,19 @@
         <v>11029866</v>
       </c>
       <c r="B19" t="s" s="8">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C19" t="s" s="8">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D19" t="s" s="8">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E19" t="s" s="8">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F19" t="s" s="8">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G19" s="10"/>
       <c r="H19" t="s" s="9">
@@ -2765,19 +2774,19 @@
         <v>11029866</v>
       </c>
       <c r="B20" t="s" s="8">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C20" t="s" s="8">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D20" t="s" s="8">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E20" t="s" s="8">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F20" t="s" s="8">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" t="s" s="9">
@@ -2806,7 +2815,7 @@
         <v>11038489</v>
       </c>
       <c r="B21" t="s" s="8">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C21" t="s" s="9">
         <v>40</v>
@@ -2818,7 +2827,7 @@
         <v>42</v>
       </c>
       <c r="F21" t="s" s="9">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="G21" s="10"/>
       <c r="H21" t="s" s="9">
@@ -2847,7 +2856,7 @@
         <v>11032259</v>
       </c>
       <c r="B22" t="s" s="8">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C22" t="s" s="9">
         <v>59</v>
@@ -2859,7 +2868,7 @@
         <v>61</v>
       </c>
       <c r="F22" t="s" s="9">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="G22" s="10"/>
       <c r="H22" t="s" s="9">
@@ -2940,19 +2949,19 @@
         <v>5</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="I1" t="s" s="2">
         <v>12</v>
       </c>
       <c r="J1" t="s" s="2">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="K1" t="s" s="2">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="L1" t="s" s="2">
         <v>14</v>
@@ -2961,13 +2970,13 @@
         <v>15</v>
       </c>
       <c r="N1" t="s" s="2">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="O1" t="s" s="2">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="P1" t="s" s="2">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="Q1" t="s" s="2">
         <v>16</v>
@@ -2976,7 +2985,7 @@
         <v>18</v>
       </c>
       <c r="S1" t="s" s="2">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" ht="13.55" customHeight="1">
@@ -3203,13 +3212,13 @@
         <v>27</v>
       </c>
       <c r="E1" t="s" s="13">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H1" t="s" s="2">
         <v>39</v>

</xml_diff>